<commit_message>
chức năng nhập xuất tồn
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DsSanPhamHetHang.xlsx
+++ b/src/main/resources/excel/DsSanPhamHetHang.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mã Sản Phẩm</t>
   </si>
@@ -86,13 +86,31 @@
   </si>
   <si>
     <t>DANH SÁCH SẢN PHẨM SẮP HẾT HÀNG</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Macbook</t>
+  </si>
+  <si>
+    <t>Ipad</t>
+  </si>
+  <si>
+    <t>Notepad</t>
+  </si>
+  <si>
+    <t>Phone Accessories</t>
+  </si>
+  <si>
+    <t>Laptop Accessories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +150,19 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +236,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +918,7 @@
     <col min="16134" max="16134" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
@@ -888,33 +926,37 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -923,8 +965,12 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -933,8 +979,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -943,8 +993,12 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -953,8 +1007,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -963,11 +1021,47 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="L8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>$N$3:$N$14</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+      <formula1>$L$3:$L$8</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>